<commit_message>
add property of skill
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Ini/HeroSkill.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Ini/HeroSkill.xlsx
@@ -1,231 +1,216 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12375" windowHeight="7905"/>
+    <workbookView windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="144525"/>
+  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Skill" type="4" refreshedVersion="0" background="1">
-    <webPr xml="1" sourceData="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlTables="1" htmlFormat="all"/>
+  <connection id="1" name="Skill" type="4" background="1" refreshedVersion="2" saveData="1">
+    <webPr parsePre="1" consecutive="1" xl2000="1" sourceData="1" xml="1" url="D:\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Ini\Skill.xml" htmlFormat="all" htmlTables="1"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
   <si>
     <t>ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>AnimaState</t>
+  </si>
+  <si>
+    <t>AtkDis</t>
+  </si>
+  <si>
+    <t>NeedTar</t>
+  </si>
+  <si>
+    <t>Hero1_Normal_1</t>
   </si>
   <si>
     <t>skill1</t>
   </si>
   <si>
-    <t>AnimaState</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AtkDis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NeedTar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>NameID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Hero1_Normal_2</t>
   </si>
   <si>
     <t>skill2</t>
   </si>
   <si>
+    <t>Hero1_Normal_3</t>
+  </si>
+  <si>
     <t>skill3</t>
   </si>
   <si>
+    <t>Hero1_Normal_4</t>
+  </si>
+  <si>
     <t>skill4</t>
   </si>
   <si>
+    <t>Hero1_Skill1</t>
+  </si>
+  <si>
     <t>skill5</t>
   </si>
   <si>
+    <t>Hero1_Skill2</t>
+  </si>
+  <si>
     <t>skill6</t>
   </si>
   <si>
+    <t>Hero1_Skill3</t>
+  </si>
+  <si>
     <t>skill7</t>
   </si>
   <si>
+    <t>Hero1_Skill4</t>
+  </si>
+  <si>
     <t>skill8</t>
   </si>
   <si>
+    <t>Hero2_Normal_1</t>
+  </si>
+  <si>
     <t>skill9</t>
   </si>
   <si>
+    <t>Hero2_Normal_2</t>
+  </si>
+  <si>
     <t>skill10</t>
   </si>
   <si>
+    <t>Hero2_Normal_3</t>
+  </si>
+  <si>
     <t>skill11</t>
   </si>
   <si>
+    <t>Hero2_Normal_4</t>
+  </si>
+  <si>
     <t>skill12</t>
   </si>
   <si>
+    <t>Hero2_Skill1</t>
+  </si>
+  <si>
     <t>skill13</t>
   </si>
   <si>
+    <t>Hero2_Skill2</t>
+  </si>
+  <si>
     <t>skill14</t>
   </si>
   <si>
+    <t>Hero2_Skill3</t>
+  </si>
+  <si>
     <t>skill15</t>
   </si>
   <si>
+    <t>Hero2_Skill4</t>
+  </si>
+  <si>
     <t>skill16</t>
   </si>
   <si>
+    <t>Hero3_Normal_1</t>
+  </si>
+  <si>
     <t>skill17</t>
   </si>
   <si>
+    <t>Hero3_Normal_2</t>
+  </si>
+  <si>
     <t>skill18</t>
   </si>
   <si>
+    <t>Hero3_Normal_3</t>
+  </si>
+  <si>
     <t>skill19</t>
   </si>
   <si>
+    <t>Hero3_Normal_4</t>
+  </si>
+  <si>
     <t>skill20</t>
   </si>
   <si>
+    <t>Hero3_Skill1</t>
+  </si>
+  <si>
     <t>skill21</t>
   </si>
   <si>
+    <t>Hero3_Skill2</t>
+  </si>
+  <si>
     <t>skill22</t>
   </si>
   <si>
+    <t>Hero3_Skill3</t>
+  </si>
+  <si>
     <t>skill23</t>
   </si>
   <si>
+    <t>Hero3_Skill4</t>
+  </si>
+  <si>
     <t>skill24</t>
-  </si>
-  <si>
-    <t>Hero1_Normal_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hero1_Normal_2</t>
-  </si>
-  <si>
-    <t>Hero1_Normal_3</t>
-  </si>
-  <si>
-    <t>Hero1_Normal_4</t>
-  </si>
-  <si>
-    <t>Hero1_Skill1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hero1_Skill2</t>
-  </si>
-  <si>
-    <t>Hero1_Skill3</t>
-  </si>
-  <si>
-    <t>Hero1_Skill4</t>
-  </si>
-  <si>
-    <t>Hero2_Normal_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hero2_Normal_2</t>
-  </si>
-  <si>
-    <t>Hero2_Normal_3</t>
-  </si>
-  <si>
-    <t>Hero2_Normal_4</t>
-  </si>
-  <si>
-    <t>Hero2_Skill1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hero2_Skill2</t>
-  </si>
-  <si>
-    <t>Hero2_Skill3</t>
-  </si>
-  <si>
-    <t>Hero2_Skill4</t>
-  </si>
-  <si>
-    <t>Hero3_Normal_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hero3_Normal_2</t>
-  </si>
-  <si>
-    <t>Hero3_Normal_3</t>
-  </si>
-  <si>
-    <t>Hero3_Normal_4</t>
-  </si>
-  <si>
-    <t>Hero3_Skill1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Hero3_Skill2</t>
-  </si>
-  <si>
-    <t>Hero3_Skill3</t>
-  </si>
-  <si>
-    <t>Hero3_Skill4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color indexed="8"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="3">
@@ -237,8 +222,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor indexed="27"/>
+        <bgColor indexed="27"/>
       </patternFill>
     </fill>
   </fills>
@@ -252,31 +237,46 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="44"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="44"/>
       </top>
       <bottom style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="44"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="44"/>
       </left>
       <right/>
       <top style="thin">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color indexed="44"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -284,124 +284,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="宋体"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/xmlMaps.xml><?xml version="1.0" encoding="utf-8"?>
-<MapInfo xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" SelectionNamespaces="">
-  <Schema ID="Schema1">
-    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
-      <xsd:element nillable="true" name="XML">
-        <xsd:complexType>
-          <xsd:sequence minOccurs="0">
-            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Object" form="unqualified">
-              <xsd:complexType>
-                <xsd:attribute name="ID" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="Name" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="NextLevelID" form="unqualified" type="xsd:string"/>
-                <xsd:attribute name="NeedMoney" form="unqualified" type="xsd:integer"/>
-                <xsd:attribute name="NeedLevel" form="unqualified" type="xsd:integer"/>
-              </xsd:complexType>
-            </xsd:element>
-          </xsd:sequence>
-        </xsd:complexType>
-      </xsd:element>
-    </xsd:schema>
-  </Schema>
-  <Map ID="1" Name="XML_映射" RootElement="XML" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
-  </Map>
-</MapInfo>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:E366" tableType="xml" totalsRowShown="0" connectionId="1">
-  <autoFilter ref="A1:E366"/>
-  <tableColumns count="5">
-    <tableColumn id="1" uniqueName="ID" name="ID" dataDxfId="0">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@ID" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="2" uniqueName="Name" name="NameID">
-      <xmlColumnPr mapId="1" xpath="/XML/Object/@Name" xmlDataType="string"/>
-    </tableColumn>
-    <tableColumn id="7" uniqueName="7" name="AnimaState"/>
-    <tableColumn id="8" uniqueName="8" name="AtkDis"/>
-    <tableColumn id="10" uniqueName="10" name="NeedTar"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -411,106 +322,106 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Cans" typeface="Euphemia"/>
         <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
         <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -522,154 +433,220 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="35000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="80000">
               <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
+          <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="50000">
+            <a:gs pos="40000">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="45000"/>
+                <a:satMod val="350000"/>
+                <a:shade val="99000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:pathLst>
+            <a:path w="21600" h="21600"/>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="0">
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:srgbClr val="9CBEE0"/>
+            </a:gs>
+            <a:gs pos="0">
+              <a:srgbClr val="BBD5F0"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="739CC3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="200000"/>
+        </a:ln>
+      </a:spPr>
+      <a:bodyPr/>
+      <a:lstStyle/>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:E366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E25"/>
+      <selection activeCell="D2" sqref="D2:D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="20.875" customWidth="1"/>
     <col min="2" max="2" width="12.125" customWidth="1"/>
@@ -677,12 +654,12 @@
     <col min="4" max="5" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -694,1435 +671,1435 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>1</v>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C2">
         <v>60</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="C3">
         <v>61</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="C4">
         <v>62</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C5">
         <v>63</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>14</v>
       </c>
       <c r="C6">
         <v>101</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="C7">
         <v>101</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>18</v>
       </c>
       <c r="C8">
         <v>101</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C9">
         <v>101</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="C10">
         <v>60</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="C11">
         <v>61</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5">
       <c r="A12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="C12">
         <v>62</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5">
       <c r="A13" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
+        <v>27</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="C13">
         <v>63</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>30</v>
       </c>
       <c r="C14">
         <v>101</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5">
       <c r="A15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>18</v>
+        <v>31</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C15">
         <v>101</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5">
       <c r="A16" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>19</v>
+        <v>33</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>34</v>
       </c>
       <c r="C16">
         <v>101</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5">
       <c r="A17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C17">
         <v>101</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="A18" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>21</v>
+        <v>37</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="C18">
         <v>60</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E18">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="A19" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>40</v>
       </c>
       <c r="C19">
         <v>61</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E19">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="A20" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>23</v>
+        <v>41</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>42</v>
       </c>
       <c r="C20">
         <v>62</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="A21" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>24</v>
+        <v>43</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C21">
         <v>63</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E21">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="A22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="C22">
         <v>101</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>26</v>
+        <v>47</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C23">
         <v>101</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>27</v>
+        <v>49</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="C24">
         <v>101</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E24">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C25">
         <v>101</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="E25">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:1">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:1">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:1">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:1">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:1">
       <c r="A30" s="3"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:1">
       <c r="A31" s="3"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:1">
       <c r="A32" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:1">
       <c r="A33" s="3"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:1">
       <c r="A34" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:1">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:1">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:1">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:1">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:1">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:1">
       <c r="A40" s="3"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:1">
       <c r="A41" s="3"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:1">
       <c r="A42" s="3"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:1">
       <c r="A43" s="3"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:1">
       <c r="A44" s="3"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:1">
       <c r="A45" s="3"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:1">
       <c r="A46" s="3"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:1">
       <c r="A47" s="3"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:1">
       <c r="A48" s="3"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:1">
       <c r="A49" s="3"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:1">
       <c r="A50" s="3"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="51" spans="1:1">
       <c r="A51" s="3"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:1">
       <c r="A52" s="3"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:1">
       <c r="A53" s="3"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="54" spans="1:1">
       <c r="A54" s="3"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="55" spans="1:1">
       <c r="A55" s="3"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="56" spans="1:1">
       <c r="A56" s="3"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="57" spans="1:1">
       <c r="A57" s="3"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="58" spans="1:1">
       <c r="A58" s="3"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="59" spans="1:1">
       <c r="A59" s="3"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="60" spans="1:1">
       <c r="A60" s="3"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="61" spans="1:1">
       <c r="A61" s="3"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="62" spans="1:1">
       <c r="A62" s="3"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="63" spans="1:1">
       <c r="A63" s="3"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="64" spans="1:1">
       <c r="A64" s="3"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="65" spans="1:1">
       <c r="A65" s="3"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="66" spans="1:1">
       <c r="A66" s="3"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="67" spans="1:1">
       <c r="A67" s="3"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="68" spans="1:1">
       <c r="A68" s="3"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="69" spans="1:1">
       <c r="A69" s="3"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="70" spans="1:1">
       <c r="A70" s="3"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="71" spans="1:1">
       <c r="A71" s="3"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="72" spans="1:1">
       <c r="A72" s="3"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="73" spans="1:1">
       <c r="A73" s="3"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="74" spans="1:1">
       <c r="A74" s="3"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="75" spans="1:1">
       <c r="A75" s="3"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="76" spans="1:1">
       <c r="A76" s="3"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="77" spans="1:1">
       <c r="A77" s="3"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="78" spans="1:1">
       <c r="A78" s="3"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="79" spans="1:1">
       <c r="A79" s="3"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="80" spans="1:1">
       <c r="A80" s="3"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="81" spans="1:1">
       <c r="A81" s="3"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="82" spans="1:1">
       <c r="A82" s="3"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="83" spans="1:1">
       <c r="A83" s="3"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="84" spans="1:1">
       <c r="A84" s="3"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="85" spans="1:1">
       <c r="A85" s="3"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="86" spans="1:1">
       <c r="A86" s="3"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="87" spans="1:1">
       <c r="A87" s="3"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="88" spans="1:1">
       <c r="A88" s="3"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="89" spans="1:1">
       <c r="A89" s="3"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="90" spans="1:1">
       <c r="A90" s="3"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="91" spans="1:1">
       <c r="A91" s="3"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="92" spans="1:1">
       <c r="A92" s="3"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="93" spans="1:1">
       <c r="A93" s="3"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="94" spans="1:1">
       <c r="A94" s="3"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="95" spans="1:1">
       <c r="A95" s="3"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="96" spans="1:1">
       <c r="A96" s="3"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="97" spans="1:1">
       <c r="A97" s="3"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="98" spans="1:1">
       <c r="A98" s="3"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="99" spans="1:1">
       <c r="A99" s="3"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="100" spans="1:1">
       <c r="A100" s="3"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="101" spans="1:1">
       <c r="A101" s="3"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="102" spans="1:1">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="103" spans="1:1">
       <c r="A103" s="3"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="104" spans="1:1">
       <c r="A104" s="3"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="105" spans="1:1">
       <c r="A105" s="3"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="106" spans="1:1">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="107" spans="1:1">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="108" spans="1:1">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="109" spans="1:1">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="110" spans="1:1">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="111" spans="1:1">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="112" spans="1:1">
       <c r="A112" s="3"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="113" spans="1:1">
       <c r="A113" s="3"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="114" spans="1:1">
       <c r="A114" s="3"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="115" spans="1:1">
       <c r="A115" s="3"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="116" spans="1:1">
       <c r="A116" s="3"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="117" spans="1:1">
       <c r="A117" s="3"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="118" spans="1:1">
       <c r="A118" s="3"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="119" spans="1:1">
       <c r="A119" s="3"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="120" spans="1:1">
       <c r="A120" s="3"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="121" spans="1:1">
       <c r="A121" s="3"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="122" spans="1:1">
       <c r="A122" s="3"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="123" spans="1:1">
       <c r="A123" s="3"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="124" spans="1:1">
       <c r="A124" s="3"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="125" spans="1:1">
       <c r="A125" s="3"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="126" spans="1:1">
       <c r="A126" s="3"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="127" spans="1:1">
       <c r="A127" s="3"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="128" spans="1:1">
       <c r="A128" s="3"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="129" spans="1:1">
       <c r="A129" s="3"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="130" spans="1:1">
       <c r="A130" s="3"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="131" spans="1:1">
       <c r="A131" s="3"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="132" spans="1:1">
       <c r="A132" s="3"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="133" spans="1:1">
       <c r="A133" s="3"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="134" spans="1:1">
       <c r="A134" s="3"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="135" spans="1:1">
       <c r="A135" s="3"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="136" spans="1:1">
       <c r="A136" s="3"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="137" spans="1:1">
       <c r="A137" s="3"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="138" spans="1:1">
       <c r="A138" s="3"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="139" spans="1:1">
       <c r="A139" s="3"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="140" spans="1:1">
       <c r="A140" s="3"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="141" spans="1:1">
       <c r="A141" s="3"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="142" spans="1:1">
       <c r="A142" s="3"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="143" spans="1:1">
       <c r="A143" s="3"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="144" spans="1:1">
       <c r="A144" s="3"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="145" spans="1:1">
       <c r="A145" s="3"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="146" spans="1:1">
       <c r="A146" s="3"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="147" spans="1:1">
       <c r="A147" s="3"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="148" spans="1:1">
       <c r="A148" s="3"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="149" spans="1:1">
       <c r="A149" s="3"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="150" spans="1:1">
       <c r="A150" s="3"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="151" spans="1:1">
       <c r="A151" s="3"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="152" spans="1:1">
       <c r="A152" s="3"/>
     </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="153" spans="1:1">
       <c r="A153" s="3"/>
     </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="154" spans="1:1">
       <c r="A154" s="3"/>
     </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="155" spans="1:1">
       <c r="A155" s="3"/>
     </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="156" spans="1:1">
       <c r="A156" s="3"/>
     </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="157" spans="1:1">
       <c r="A157" s="3"/>
     </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="158" spans="1:1">
       <c r="A158" s="3"/>
     </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="159" spans="1:1">
       <c r="A159" s="3"/>
     </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="160" spans="1:1">
       <c r="A160" s="3"/>
     </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="161" spans="1:1">
       <c r="A161" s="3"/>
     </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="162" spans="1:1">
       <c r="A162" s="3"/>
     </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="163" spans="1:1">
       <c r="A163" s="3"/>
     </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="164" spans="1:1">
       <c r="A164" s="3"/>
     </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="165" spans="1:1">
       <c r="A165" s="3"/>
     </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="166" spans="1:1">
       <c r="A166" s="3"/>
     </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="167" spans="1:1">
       <c r="A167" s="3"/>
     </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="168" spans="1:1">
       <c r="A168" s="3"/>
     </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="169" spans="1:1">
       <c r="A169" s="3"/>
     </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="170" spans="1:1">
       <c r="A170" s="3"/>
     </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="171" spans="1:1">
       <c r="A171" s="3"/>
     </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="172" spans="1:1">
       <c r="A172" s="3"/>
     </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="173" spans="1:1">
       <c r="A173" s="3"/>
     </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="174" spans="1:1">
       <c r="A174" s="3"/>
     </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="175" spans="1:1">
       <c r="A175" s="3"/>
     </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="176" spans="1:1">
       <c r="A176" s="3"/>
     </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="177" spans="1:1">
       <c r="A177" s="3"/>
     </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="178" spans="1:1">
       <c r="A178" s="3"/>
     </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="179" spans="1:1">
       <c r="A179" s="3"/>
     </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="180" spans="1:1">
       <c r="A180" s="3"/>
     </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="181" spans="1:1">
       <c r="A181" s="3"/>
     </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="182" spans="1:1">
       <c r="A182" s="3"/>
     </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="183" spans="1:1">
       <c r="A183" s="3"/>
     </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="184" spans="1:1">
       <c r="A184" s="3"/>
     </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="185" spans="1:1">
       <c r="A185" s="3"/>
     </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="186" spans="1:1">
       <c r="A186" s="3"/>
     </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="187" spans="1:1">
       <c r="A187" s="3"/>
     </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="188" spans="1:1">
       <c r="A188" s="3"/>
     </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="189" spans="1:1">
       <c r="A189" s="3"/>
     </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="190" spans="1:1">
       <c r="A190" s="3"/>
     </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="191" spans="1:1">
       <c r="A191" s="3"/>
     </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="192" spans="1:1">
       <c r="A192" s="3"/>
     </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="193" spans="1:1">
       <c r="A193" s="3"/>
     </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="194" spans="1:1">
       <c r="A194" s="3"/>
     </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="195" spans="1:1">
       <c r="A195" s="3"/>
     </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="196" spans="1:1">
       <c r="A196" s="3"/>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="197" spans="1:1">
       <c r="A197" s="3"/>
     </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="198" spans="1:1">
       <c r="A198" s="3"/>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="199" spans="1:1">
       <c r="A199" s="3"/>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="200" spans="1:1">
       <c r="A200" s="3"/>
     </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="201" spans="1:1">
       <c r="A201" s="3"/>
     </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="202" spans="1:1">
       <c r="A202" s="3"/>
     </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="203" spans="1:1">
       <c r="A203" s="3"/>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="204" spans="1:1">
       <c r="A204" s="3"/>
     </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="205" spans="1:1">
       <c r="A205" s="3"/>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="206" spans="1:1">
       <c r="A206" s="3"/>
     </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="207" spans="1:1">
       <c r="A207" s="3"/>
     </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="208" spans="1:1">
       <c r="A208" s="3"/>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="209" spans="1:1">
       <c r="A209" s="3"/>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="210" spans="1:1">
       <c r="A210" s="3"/>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="211" spans="1:1">
       <c r="A211" s="3"/>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="212" spans="1:1">
       <c r="A212" s="3"/>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="213" spans="1:1">
       <c r="A213" s="3"/>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="214" spans="1:1">
       <c r="A214" s="3"/>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="215" spans="1:1">
       <c r="A215" s="3"/>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="216" spans="1:1">
       <c r="A216" s="3"/>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="217" spans="1:1">
       <c r="A217" s="3"/>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="218" spans="1:1">
       <c r="A218" s="3"/>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="219" spans="1:1">
       <c r="A219" s="3"/>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="220" spans="1:1">
       <c r="A220" s="3"/>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="221" spans="1:1">
       <c r="A221" s="3"/>
     </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="222" spans="1:1">
       <c r="A222" s="3"/>
     </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="223" spans="1:1">
       <c r="A223" s="3"/>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="224" spans="1:1">
       <c r="A224" s="3"/>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="225" spans="1:1">
       <c r="A225" s="3"/>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="226" spans="1:1">
       <c r="A226" s="3"/>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="227" spans="1:1">
       <c r="A227" s="3"/>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="228" spans="1:1">
       <c r="A228" s="3"/>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="229" spans="1:1">
       <c r="A229" s="3"/>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="230" spans="1:1">
       <c r="A230" s="3"/>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="231" spans="1:1">
       <c r="A231" s="3"/>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="232" spans="1:1">
       <c r="A232" s="3"/>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="233" spans="1:1">
       <c r="A233" s="3"/>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="234" spans="1:1">
       <c r="A234" s="3"/>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="235" spans="1:1">
       <c r="A235" s="3"/>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="236" spans="1:1">
       <c r="A236" s="3"/>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="237" spans="1:1">
       <c r="A237" s="3"/>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="238" spans="1:1">
       <c r="A238" s="3"/>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="239" spans="1:1">
       <c r="A239" s="3"/>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="240" spans="1:1">
       <c r="A240" s="3"/>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="241" spans="1:1">
       <c r="A241" s="3"/>
     </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="242" spans="1:1">
       <c r="A242" s="3"/>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="243" spans="1:1">
       <c r="A243" s="3"/>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="244" spans="1:1">
       <c r="A244" s="3"/>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="245" spans="1:1">
       <c r="A245" s="3"/>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="246" spans="1:1">
       <c r="A246" s="3"/>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="247" spans="1:1">
       <c r="A247" s="3"/>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="248" spans="1:1">
       <c r="A248" s="3"/>
     </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="249" spans="1:1">
       <c r="A249" s="3"/>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="250" spans="1:1">
       <c r="A250" s="3"/>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="251" spans="1:1">
       <c r="A251" s="3"/>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="252" spans="1:1">
       <c r="A252" s="3"/>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="253" spans="1:1">
       <c r="A253" s="3"/>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="254" spans="1:1">
       <c r="A254" s="3"/>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="255" spans="1:1">
       <c r="A255" s="3"/>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="256" spans="1:1">
       <c r="A256" s="3"/>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="257" spans="1:1">
       <c r="A257" s="3"/>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="258" spans="1:1">
       <c r="A258" s="3"/>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="259" spans="1:1">
       <c r="A259" s="3"/>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="260" spans="1:1">
       <c r="A260" s="3"/>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="261" spans="1:1">
       <c r="A261" s="3"/>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="262" spans="1:1">
       <c r="A262" s="3"/>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="263" spans="1:1">
       <c r="A263" s="3"/>
     </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="264" spans="1:1">
       <c r="A264" s="3"/>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="265" spans="1:1">
       <c r="A265" s="3"/>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="266" spans="1:1">
       <c r="A266" s="3"/>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="267" spans="1:1">
       <c r="A267" s="3"/>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="268" spans="1:1">
       <c r="A268" s="3"/>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="269" spans="1:1">
       <c r="A269" s="3"/>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="270" spans="1:1">
       <c r="A270" s="3"/>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="271" spans="1:1">
       <c r="A271" s="3"/>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="272" spans="1:1">
       <c r="A272" s="3"/>
     </row>
-    <row r="273" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="273" spans="1:1">
       <c r="A273" s="3"/>
     </row>
-    <row r="274" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="274" spans="1:1">
       <c r="A274" s="3"/>
     </row>
-    <row r="275" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="275" spans="1:1">
       <c r="A275" s="3"/>
     </row>
-    <row r="276" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="276" spans="1:1">
       <c r="A276" s="3"/>
     </row>
-    <row r="277" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="277" spans="1:1">
       <c r="A277" s="3"/>
     </row>
-    <row r="278" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="278" spans="1:1">
       <c r="A278" s="3"/>
     </row>
-    <row r="279" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="279" spans="1:1">
       <c r="A279" s="3"/>
     </row>
-    <row r="280" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="280" spans="1:1">
       <c r="A280" s="3"/>
     </row>
-    <row r="281" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="281" spans="1:1">
       <c r="A281" s="3"/>
     </row>
-    <row r="282" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="282" spans="1:1">
       <c r="A282" s="3"/>
     </row>
-    <row r="283" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="283" spans="1:1">
       <c r="A283" s="3"/>
     </row>
-    <row r="284" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="284" spans="1:1">
       <c r="A284" s="3"/>
     </row>
-    <row r="285" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="285" spans="1:1">
       <c r="A285" s="3"/>
     </row>
-    <row r="286" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="286" spans="1:1">
       <c r="A286" s="3"/>
     </row>
-    <row r="287" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="287" spans="1:1">
       <c r="A287" s="3"/>
     </row>
-    <row r="288" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="288" spans="1:1">
       <c r="A288" s="3"/>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="289" spans="1:1">
       <c r="A289" s="3"/>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="290" spans="1:1">
       <c r="A290" s="3"/>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="291" spans="1:1">
       <c r="A291" s="3"/>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="292" spans="1:1">
       <c r="A292" s="3"/>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="293" spans="1:1">
       <c r="A293" s="3"/>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="294" spans="1:1">
       <c r="A294" s="3"/>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="295" spans="1:1">
       <c r="A295" s="3"/>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="296" spans="1:1">
       <c r="A296" s="3"/>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="297" spans="1:1">
       <c r="A297" s="3"/>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="298" spans="1:1">
       <c r="A298" s="3"/>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="299" spans="1:1">
       <c r="A299" s="3"/>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="300" spans="1:1">
       <c r="A300" s="3"/>
     </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="301" spans="1:1">
       <c r="A301" s="3"/>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="302" spans="1:1">
       <c r="A302" s="3"/>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="303" spans="1:1">
       <c r="A303" s="3"/>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="304" spans="1:1">
       <c r="A304" s="3"/>
     </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="305" spans="1:1">
       <c r="A305" s="3"/>
     </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="306" spans="1:1">
       <c r="A306" s="3"/>
     </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="307" spans="1:1">
       <c r="A307" s="3"/>
     </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="308" spans="1:1">
       <c r="A308" s="3"/>
     </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="309" spans="1:1">
       <c r="A309" s="3"/>
     </row>
-    <row r="310" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="310" spans="1:1">
       <c r="A310" s="3"/>
     </row>
-    <row r="311" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="311" spans="1:1">
       <c r="A311" s="3"/>
     </row>
-    <row r="312" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="312" spans="1:1">
       <c r="A312" s="3"/>
     </row>
-    <row r="313" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="313" spans="1:1">
       <c r="A313" s="3"/>
     </row>
-    <row r="314" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="314" spans="1:1">
       <c r="A314" s="3"/>
     </row>
-    <row r="315" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="315" spans="1:1">
       <c r="A315" s="3"/>
     </row>
-    <row r="316" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="316" spans="1:1">
       <c r="A316" s="3"/>
     </row>
-    <row r="317" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="317" spans="1:1">
       <c r="A317" s="3"/>
     </row>
-    <row r="318" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="318" spans="1:1">
       <c r="A318" s="3"/>
     </row>
-    <row r="319" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="319" spans="1:1">
       <c r="A319" s="3"/>
     </row>
-    <row r="320" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="320" spans="1:1">
       <c r="A320" s="3"/>
     </row>
-    <row r="321" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="321" spans="1:1">
       <c r="A321" s="3"/>
     </row>
-    <row r="322" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="322" spans="1:1">
       <c r="A322" s="3"/>
     </row>
-    <row r="323" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="323" spans="1:1">
       <c r="A323" s="3"/>
     </row>
-    <row r="324" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="324" spans="1:1">
       <c r="A324" s="3"/>
     </row>
-    <row r="325" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="325" spans="1:1">
       <c r="A325" s="3"/>
     </row>
-    <row r="326" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="326" spans="1:1">
       <c r="A326" s="3"/>
     </row>
-    <row r="327" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="327" spans="1:1">
       <c r="A327" s="3"/>
     </row>
-    <row r="328" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="328" spans="1:1">
       <c r="A328" s="3"/>
     </row>
-    <row r="329" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="329" spans="1:1">
       <c r="A329" s="3"/>
     </row>
-    <row r="330" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="330" spans="1:1">
       <c r="A330" s="3"/>
     </row>
-    <row r="331" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="331" spans="1:1">
       <c r="A331" s="3"/>
     </row>
-    <row r="332" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="332" spans="1:1">
       <c r="A332" s="3"/>
     </row>
-    <row r="333" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="333" spans="1:1">
       <c r="A333" s="3"/>
     </row>
-    <row r="334" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="334" spans="1:1">
       <c r="A334" s="3"/>
     </row>
-    <row r="335" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="335" spans="1:1">
       <c r="A335" s="3"/>
     </row>
-    <row r="336" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="336" spans="1:1">
       <c r="A336" s="3"/>
     </row>
-    <row r="337" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="337" spans="1:1">
       <c r="A337" s="3"/>
     </row>
-    <row r="338" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="338" spans="1:1">
       <c r="A338" s="3"/>
     </row>
-    <row r="339" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="339" spans="1:1">
       <c r="A339" s="3"/>
     </row>
-    <row r="340" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="340" spans="1:1">
       <c r="A340" s="3"/>
     </row>
-    <row r="341" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="341" spans="1:1">
       <c r="A341" s="3"/>
     </row>
-    <row r="342" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="342" spans="1:1">
       <c r="A342" s="3"/>
     </row>
-    <row r="343" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="343" spans="1:1">
       <c r="A343" s="3"/>
     </row>
-    <row r="344" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="344" spans="1:1">
       <c r="A344" s="3"/>
     </row>
-    <row r="345" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="345" spans="1:1">
       <c r="A345" s="3"/>
     </row>
-    <row r="346" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="346" spans="1:1">
       <c r="A346" s="3"/>
     </row>
-    <row r="347" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="347" spans="1:1">
       <c r="A347" s="3"/>
     </row>
-    <row r="348" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="348" spans="1:1">
       <c r="A348" s="3"/>
     </row>
-    <row r="349" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="349" spans="1:1">
       <c r="A349" s="3"/>
     </row>
-    <row r="350" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="350" spans="1:1">
       <c r="A350" s="3"/>
     </row>
-    <row r="351" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="351" spans="1:1">
       <c r="A351" s="3"/>
     </row>
-    <row r="352" spans="1:1" x14ac:dyDescent="0.15">
+    <row r="352" spans="1:1">
       <c r="A352" s="3"/>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="353" spans="1:1">
       <c r="A353" s="3"/>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="354" spans="1:1">
       <c r="A354" s="3"/>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="355" spans="1:1">
       <c r="A355" s="3"/>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="356" spans="1:1">
       <c r="A356" s="3"/>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="357" spans="1:1">
       <c r="A357" s="3"/>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="358" spans="1:1">
       <c r="A358" s="3"/>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="359" spans="1:1">
       <c r="A359" s="3"/>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="360" spans="1:1">
       <c r="A360" s="3"/>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="361" spans="1:1">
       <c r="A361" s="3"/>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="362" spans="1:1">
       <c r="A362" s="3"/>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="363" spans="1:1">
       <c r="A363" s="3"/>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="364" spans="1:1">
       <c r="A364" s="3"/>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="365" spans="1:1">
       <c r="A365" s="3"/>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="366" spans="1:5">
       <c r="A366" s="4"/>
       <c r="B366" s="5"/>
       <c r="C366" s="5"/>
@@ -2130,11 +2107,8 @@
       <c r="E366" s="5"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>